<commit_message>
update user logout feature
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/requestBodyDetails.xlsx
+++ b/src/test/resources/testData/requestBodyDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anil.basudkar\eclipse-workspace\T7_RestlessCoders_DieticianAPI_Hackathon_nov_2023\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D4B165-EC40-41A0-8385-6C37E930BE39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20226C11-93E1-430F-99FC-3807A0E8FA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{0E5AE6ED-B2BD-49D4-8895-9B2C6FFBF544}"/>
   </bookViews>
@@ -562,7 +562,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,7 +574,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>96</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>